<commit_message>
attendance sheet download set up
</commit_message>
<xml_diff>
--- a/media/Attendance/sheet_2.xlsx
+++ b/media/Attendance/sheet_2.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2021/1/20</t>
+          <t>2021/1/15</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -465,6 +465,102 @@
         </is>
       </c>
       <c r="B3" t="inlineStr">
+        <is>
+          <t>2021-01-15 09:20:00.484737+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2021-01-15 11:02:48.016808+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2021-01-19 14:56:54.059903+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2021-01-19 14:58:27.089588+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2021-01-19 14:59:06.707655+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2021-01-19 15:00:43.456282+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2021-01-19 15:03:03.286919+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2021-01-19 15:09:10.796135+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Muskan Vaswan</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>2021-01-20 07:58:50.521689+00:00</t>
         </is>

</xml_diff>